<commit_message>
corretta immatricolazione con produzione
</commit_message>
<xml_diff>
--- a/db-cars.xlsx
+++ b/db-cars.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Cilindrata</t>
   </si>
   <si>
-    <t xml:space="preserve">Anno di Immatricolazione</t>
+    <t xml:space="preserve">Anno di Produzione</t>
   </si>
   <si>
     <t xml:space="preserve">Porte</t>
@@ -94,6 +94,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -114,12 +115,14 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,19 +215,19 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="26.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="23.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="17.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="11.52"/>
   </cols>
   <sheetData>

</xml_diff>